<commit_message>
Fix HT model underfitting
</commit_message>
<xml_diff>
--- a/models/predict/25preds ET.xlsx
+++ b/models/predict/25preds ET.xlsx
@@ -8,27 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Very old laptop\Betting\urc-score-prediction\models\predict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87409A06-7ADC-492C-BBF5-A79507CE347E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1F2B0078-80AE-456E-A8E9-C02E25983410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D7EAA4F9-AA32-4163-AF29-C819E165A0FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{FD8309E1-E492-425F-A2D1-7E75CB5CC2DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="25preds_et - Copy" sheetId="1" r:id="rId1"/>
+    <sheet name="25preds_et" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -718,6 +705,7 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -759,57 +747,56 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="42" builtinId="5"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1140,18 +1127,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831461E8-EE33-4DF6-9A1E-58EC07110A41}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC22FF06-2196-4D9E-BA9C-AC0B965EF634}">
   <dimension ref="A1:Y145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="7" max="7" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.36328125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1232,10 +1215,10 @@
         <v>8.1548483467512902</v>
       </c>
       <c r="C2">
-        <v>11.2741666666666</v>
+        <v>7.5391666666666604</v>
       </c>
       <c r="D2">
-        <v>11.939166666666599</v>
+        <v>6.2850000000000001</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -1306,10 +1289,10 @@
         <v>13.9939204608096</v>
       </c>
       <c r="C3">
-        <v>10.362500000000001</v>
+        <v>12.3808333333333</v>
       </c>
       <c r="D3">
-        <v>12.005000000000001</v>
+        <v>12.04</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -1380,10 +1363,10 @@
         <v>14.852330766435401</v>
       </c>
       <c r="C4">
-        <v>10.386666666666599</v>
+        <v>12.37</v>
       </c>
       <c r="D4">
-        <v>11.9683333333333</v>
+        <v>10.6625</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
@@ -1454,10 +1437,10 @@
         <v>31.981516683316698</v>
       </c>
       <c r="C5">
-        <v>13.181666666666599</v>
+        <v>18.074166666666599</v>
       </c>
       <c r="D5">
-        <v>12.570833333333301</v>
+        <v>16.199166666666599</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
@@ -1528,10 +1511,10 @@
         <v>22.440440365633901</v>
       </c>
       <c r="C6">
-        <v>12.8541666666666</v>
+        <v>15.4308333333333</v>
       </c>
       <c r="D6">
-        <v>12.265833333333299</v>
+        <v>12.011666666666599</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
@@ -1599,13 +1582,13 @@
         <v>18.221212426380799</v>
       </c>
       <c r="B7">
-        <v>29.520833339617901</v>
+        <v>29.520833339617798</v>
       </c>
       <c r="C7">
-        <v>12.74</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="D7">
-        <v>12.220833333333299</v>
+        <v>14.68</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
@@ -1676,10 +1659,10 @@
         <v>18.1077240638243</v>
       </c>
       <c r="C8">
-        <v>10.344166666666601</v>
+        <v>11.8716666666666</v>
       </c>
       <c r="D8">
-        <v>12.091666666666599</v>
+        <v>12.22</v>
       </c>
       <c r="E8" t="s">
         <v>46</v>
@@ -1750,10 +1733,10 @@
         <v>13.821031932671101</v>
       </c>
       <c r="C9">
-        <v>10.4158333333333</v>
+        <v>13.9166666666666</v>
       </c>
       <c r="D9">
-        <v>11.9125</v>
+        <v>6.0333333333333297</v>
       </c>
       <c r="E9" t="s">
         <v>49</v>
@@ -1862,10 +1845,10 @@
         <v>8.4317031086560501</v>
       </c>
       <c r="C11">
-        <v>11.328333333333299</v>
+        <v>7.55416666666666</v>
       </c>
       <c r="D11">
-        <v>12.000833333333301</v>
+        <v>6.5233333333333299</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
@@ -1924,7 +1907,7 @@
         <v>Home</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Y11:Y42" si="1">IF(W11=X11,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1936,10 +1919,10 @@
         <v>19.3752465798703</v>
       </c>
       <c r="C12">
-        <v>11.147500000000001</v>
+        <v>11.803333333333301</v>
       </c>
       <c r="D12">
-        <v>12.074999999999999</v>
+        <v>15.365</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -1998,7 +1981,7 @@
         <v>Home</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2048,10 +2031,10 @@
         <v>21.125016326019999</v>
       </c>
       <c r="C14">
-        <v>10.3375</v>
+        <v>10.5283333333333</v>
       </c>
       <c r="D14">
-        <v>12.092499999999999</v>
+        <v>13.1183333333333</v>
       </c>
       <c r="E14" t="s">
         <v>50</v>
@@ -2110,7 +2093,7 @@
         <v>Home</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Y14:Y42" si="2">IF(W14=X14,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2122,10 +2105,10 @@
         <v>29.905344475540701</v>
       </c>
       <c r="C15">
-        <v>12.754166666666601</v>
+        <v>18.0066666666666</v>
       </c>
       <c r="D15">
-        <v>11.0725</v>
+        <v>14.209166666666601</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>
@@ -2184,7 +2167,7 @@
         <v>Home</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2196,10 +2179,10 @@
         <v>18.9926310677325</v>
       </c>
       <c r="C16">
-        <v>10.865833333333301</v>
+        <v>8.5733333333333306</v>
       </c>
       <c r="D16">
-        <v>11.643333333333301</v>
+        <v>9.7491666666666603</v>
       </c>
       <c r="E16" t="s">
         <v>43</v>
@@ -2258,7 +2241,7 @@
         <v>Home</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2270,10 +2253,10 @@
         <v>21.489897687478699</v>
       </c>
       <c r="C17">
-        <v>12.7</v>
+        <v>14.289166666666601</v>
       </c>
       <c r="D17">
-        <v>12.2</v>
+        <v>9.6724999999999994</v>
       </c>
       <c r="E17" t="s">
         <v>37</v>
@@ -2332,7 +2315,7 @@
         <v>Home</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2344,10 +2327,10 @@
         <v>22.1654583903283</v>
       </c>
       <c r="C18">
-        <v>10.281666666666601</v>
+        <v>10.7116666666666</v>
       </c>
       <c r="D18">
-        <v>12.858333333333301</v>
+        <v>13.897500000000001</v>
       </c>
       <c r="E18" t="s">
         <v>43</v>
@@ -2406,7 +2389,7 @@
         <v>Away</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2418,10 +2401,10 @@
         <v>31.522781628257299</v>
       </c>
       <c r="C19">
-        <v>10.3041666666666</v>
+        <v>1.98166666666666</v>
       </c>
       <c r="D19">
-        <v>12.0908333333333</v>
+        <v>14.5541666666666</v>
       </c>
       <c r="E19" t="s">
         <v>42</v>
@@ -2480,7 +2463,7 @@
         <v>Away</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2492,10 +2475,10 @@
         <v>18.122331377889601</v>
       </c>
       <c r="C20">
-        <v>12.733333333333301</v>
+        <v>16.3258333333333</v>
       </c>
       <c r="D20">
-        <v>12.345000000000001</v>
+        <v>10.376666666666599</v>
       </c>
       <c r="E20" t="s">
         <v>50</v>
@@ -2554,7 +2537,7 @@
         <v>Home</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2563,13 +2546,13 @@
         <v>25.7891336076197</v>
       </c>
       <c r="B21">
-        <v>17.1945913898805</v>
+        <v>17.1945913898806</v>
       </c>
       <c r="C21">
-        <v>11.725</v>
+        <v>12.4825</v>
       </c>
       <c r="D21">
-        <v>12.7116666666666</v>
+        <v>8.4866666666666593</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -2628,7 +2611,7 @@
         <v>Home</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2640,10 +2623,10 @@
         <v>12.5353789408659</v>
       </c>
       <c r="C22">
-        <v>12.5058333333333</v>
+        <v>13.3433333333333</v>
       </c>
       <c r="D22">
-        <v>11.8816666666666</v>
+        <v>7.0341666666666596</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -2702,7 +2685,7 @@
         <v>Home</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2714,10 +2697,10 @@
         <v>15.959216922247199</v>
       </c>
       <c r="C23">
-        <v>12.3508333333333</v>
+        <v>20.816666666666599</v>
       </c>
       <c r="D23">
-        <v>12.0991666666666</v>
+        <v>15.3125</v>
       </c>
       <c r="E23" t="s">
         <v>21</v>
@@ -2776,7 +2759,7 @@
         <v>Home</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2788,10 +2771,10 @@
         <v>15.071069336525399</v>
       </c>
       <c r="C24">
-        <v>10.4158333333333</v>
+        <v>8.3149999999999995</v>
       </c>
       <c r="D24">
-        <v>11.8891666666666</v>
+        <v>8.7541666666666593</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
@@ -2850,7 +2833,7 @@
         <v>Home</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2862,10 +2845,10 @@
         <v>14.0104277448654</v>
       </c>
       <c r="C25">
-        <v>12.387499999999999</v>
+        <v>11.9541666666666</v>
       </c>
       <c r="D25">
-        <v>10.8725</v>
+        <v>9.9891666666666605</v>
       </c>
       <c r="E25" t="s">
         <v>46</v>
@@ -2924,7 +2907,7 @@
         <v>Home</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2936,10 +2919,10 @@
         <v>11.098930778269899</v>
       </c>
       <c r="C26">
-        <v>12.42</v>
+        <v>15.7183333333333</v>
       </c>
       <c r="D26">
-        <v>10.8183333333333</v>
+        <v>4.3841666666666601</v>
       </c>
       <c r="E26" t="s">
         <v>38</v>
@@ -2998,7 +2981,7 @@
         <v>Home</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3010,10 +2993,10 @@
         <v>19.2194444933947</v>
       </c>
       <c r="C27">
-        <v>10.3466666666666</v>
+        <v>7.7066666666666599</v>
       </c>
       <c r="D27">
-        <v>12.03</v>
+        <v>8.7633333333333301</v>
       </c>
       <c r="E27" t="s">
         <v>49</v>
@@ -3072,7 +3055,7 @@
         <v>Home</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3084,10 +3067,10 @@
         <v>20.142580040200802</v>
       </c>
       <c r="C28">
-        <v>10.3041666666666</v>
+        <v>8.0933333333333302</v>
       </c>
       <c r="D28">
-        <v>12.0908333333333</v>
+        <v>14.4433333333333</v>
       </c>
       <c r="E28" t="s">
         <v>26</v>
@@ -3146,7 +3129,7 @@
         <v>Home</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3158,10 +3141,10 @@
         <v>22.644647486362899</v>
       </c>
       <c r="C29">
-        <v>12.8183333333333</v>
+        <v>11.6416666666666</v>
       </c>
       <c r="D29">
-        <v>12.316666666666601</v>
+        <v>8.8783333333333303</v>
       </c>
       <c r="E29" t="s">
         <v>47</v>
@@ -3220,7 +3203,7 @@
         <v>Home</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3232,10 +3215,10 @@
         <v>27.2492839840715</v>
       </c>
       <c r="C30">
-        <v>12.6758333333333</v>
+        <v>12.1241666666666</v>
       </c>
       <c r="D30">
-        <v>12.910833333333301</v>
+        <v>17.273333333333301</v>
       </c>
       <c r="E30" t="s">
         <v>30</v>
@@ -3294,7 +3277,7 @@
         <v>Home</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3306,10 +3289,10 @@
         <v>23.708417908679099</v>
       </c>
       <c r="C31">
-        <v>11.765000000000001</v>
+        <v>14.220833333333299</v>
       </c>
       <c r="D31">
-        <v>13.08</v>
+        <v>16.739999999999998</v>
       </c>
       <c r="E31" t="s">
         <v>21</v>
@@ -3368,7 +3351,7 @@
         <v>Away</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3380,10 +3363,10 @@
         <v>28.794936266138599</v>
       </c>
       <c r="C32">
-        <v>10.796666666666599</v>
+        <v>10.101666666666601</v>
       </c>
       <c r="D32">
-        <v>12.015000000000001</v>
+        <v>12.1516666666666</v>
       </c>
       <c r="E32" t="s">
         <v>37</v>
@@ -3442,7 +3425,7 @@
         <v>Away</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3454,10 +3437,10 @@
         <v>26.301198753967899</v>
       </c>
       <c r="C33">
-        <v>10.681666666666599</v>
+        <v>9.5</v>
       </c>
       <c r="D33">
-        <v>12.894166666666599</v>
+        <v>14.758333333333301</v>
       </c>
       <c r="E33" t="s">
         <v>33</v>
@@ -3516,7 +3499,7 @@
         <v>Away</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3528,10 +3511,10 @@
         <v>14.217243231747901</v>
       </c>
       <c r="C34">
-        <v>10.4158333333333</v>
+        <v>8.6983333333333306</v>
       </c>
       <c r="D34">
-        <v>11.8891666666666</v>
+        <v>7.4858333333333302</v>
       </c>
       <c r="E34" t="s">
         <v>29</v>
@@ -3590,7 +3573,7 @@
         <v>Home</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3602,10 +3585,10 @@
         <v>26.865785214785198</v>
       </c>
       <c r="C35">
-        <v>13.0858333333333</v>
+        <v>13.5591666666666</v>
       </c>
       <c r="D35">
-        <v>12.4975</v>
+        <v>15.584166666666601</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
@@ -3664,7 +3647,7 @@
         <v>Home</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3676,10 +3659,10 @@
         <v>22.7280631465756</v>
       </c>
       <c r="C36">
-        <v>13.0716666666666</v>
+        <v>14.5691666666666</v>
       </c>
       <c r="D36">
-        <v>12.8008333333333</v>
+        <v>14.1833333333333</v>
       </c>
       <c r="E36" t="s">
         <v>30</v>
@@ -3738,22 +3721,22 @@
         <v>Home</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>36.570265762019297</v>
+        <v>36.570265762019197</v>
       </c>
       <c r="B37">
         <v>16.9644507558972</v>
       </c>
       <c r="C37">
-        <v>12.452500000000001</v>
+        <v>20.884166666666601</v>
       </c>
       <c r="D37">
-        <v>11.8158333333333</v>
+        <v>15.6225</v>
       </c>
       <c r="E37" t="s">
         <v>21</v>
@@ -3812,7 +3795,7 @@
         <v>Home</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3824,10 +3807,10 @@
         <v>27.579103739596501</v>
       </c>
       <c r="C38">
-        <v>12.362500000000001</v>
+        <v>13.8116666666666</v>
       </c>
       <c r="D38">
-        <v>10.900833333333299</v>
+        <v>9.2916666666666607</v>
       </c>
       <c r="E38" t="s">
         <v>50</v>
@@ -3886,7 +3869,7 @@
         <v>Away</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3898,10 +3881,10 @@
         <v>19.193751496170002</v>
       </c>
       <c r="C39">
-        <v>12.452500000000001</v>
+        <v>9.8066666666666595</v>
       </c>
       <c r="D39">
-        <v>11.8158333333333</v>
+        <v>12.101666666666601</v>
       </c>
       <c r="E39" t="s">
         <v>26</v>
@@ -3960,7 +3943,7 @@
         <v>Home</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3972,10 +3955,10 @@
         <v>15.5280843170975</v>
       </c>
       <c r="C40">
-        <v>10.886666666666599</v>
+        <v>10.348333333333301</v>
       </c>
       <c r="D40">
-        <v>11.879166666666601</v>
+        <v>12.0891666666666</v>
       </c>
       <c r="E40" t="s">
         <v>43</v>
@@ -4034,7 +4017,7 @@
         <v>Home</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -4046,10 +4029,10 @@
         <v>15.9903374518251</v>
       </c>
       <c r="C41">
-        <v>12.4191666666666</v>
+        <v>12.2383333333333</v>
       </c>
       <c r="D41">
-        <v>10.816666666666601</v>
+        <v>11.011666666666599</v>
       </c>
       <c r="E41" t="s">
         <v>46</v>
@@ -4108,7 +4091,7 @@
         <v>Home</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>